<commit_message>
cosmetic adjustments to Filter API spreadsheet
</commit_message>
<xml_diff>
--- a/notes/Filter API.xlsx
+++ b/notes/Filter API.xlsx
@@ -250,7 +250,25 @@
   </si>
   <si>
     <r>
-      <t>getFilter(columnIndexOrName, options)</t>
+      <t>setGlobalFilterCaseSensitivity(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>isSensitive</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
     </r>
     <r>
       <rPr>
@@ -260,7 +278,30 @@
         <color theme="1"/>
         <rFont val="Lucida Console"/>
       </rPr>
-      <t>3</t>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>getFilter(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>columnIndexOrName, options</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
     </r>
   </si>
   <si>
@@ -269,6 +310,7 @@
     </r>
     <r>
       <rPr>
+        <i/>
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Lucida Console"/>
@@ -292,20 +334,110 @@
         <color theme="1"/>
         <rFont val="Lucida Console"/>
       </rPr>
-      <t>2,3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>setFilter(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>columnIndexOrName, state, options</t>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>getTableFilter(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>options</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>setTableFitler(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>state, options</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>setGlobalFilter(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>filter</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>setGlobalFilter(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>filter</t>
     </r>
     <r>
       <rPr>
@@ -339,6 +471,52 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>setCaseSensitivity(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>isSensitive</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>setTableFitler(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>state, options</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -347,44 +525,21 @@
         <color theme="1"/>
         <rFont val="Lucida Console"/>
       </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>getFilter(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>columnIndexOrName, options</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>setFilter(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>columnIndexOrName, state, options</t>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>setGlobalFilter(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>filter</t>
     </r>
     <r>
       <rPr>
@@ -403,68 +558,12 @@
         <color theme="1"/>
         <rFont val="Lucida Console"/>
       </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>getTableFilter(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>options</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>setTableFitler(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>state, options</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>setGlobalFilter(</t>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>set(</t>
     </r>
     <r>
       <rPr>
@@ -477,27 +576,16 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>setGlobalFilter(</t>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>get(</t>
     </r>
     <r>
       <rPr>
@@ -520,163 +608,6 @@
   </si>
   <si>
     <r>
-      <t>setGlobalFilterCaseSensitivity(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>isSensitive</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>setCaseSensitivity(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>isSensitive</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>setTableFitler(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>state, options</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>setGlobalFilter(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>filter</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>set(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>filter</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>get(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>filter</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>test(</t>
     </r>
     <r>
@@ -696,38 +627,6 @@
         <rFont val="Lucida Console"/>
       </rPr>
       <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>setColumnFilterState(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>columnIndexOrName, state, options</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Lucida Console"/>
-      </rPr>
-      <t>4,5</t>
     </r>
   </si>
   <si>
@@ -1099,6 +998,128 @@
         <rFont val="Lucida Console"/>
       </rPr>
       <t xml:space="preserve"> 'SQL'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>getFilter(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>columnIndexOrName, options</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>setColumnFilterState(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>columnIndexOrName, state, options</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>4,5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>setFilter(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>columnIndexOrName, state, options</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>2,3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>setFilter(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>columnIndexOrName, state, options</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
     </r>
   </si>
 </sst>
@@ -1761,11 +1782,11 @@
         <v>23</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1785,7 +1806,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G4" s="26" t="s">
         <v>4</v>
@@ -1793,19 +1814,19 @@
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G5" s="29" t="s">
         <v>4</v>
@@ -1816,16 +1837,16 @@
         <v>16</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
@@ -1848,7 +1869,7 @@
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1867,7 +1888,7 @@
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1875,38 +1896,38 @@
         <v>12</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="28" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1914,38 +1935,38 @@
         <v>13</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="28" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1965,10 +1986,10 @@
         <v>4</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1997,7 +2018,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
jsdoc edits for filter API; added get/setColumnFilters()
</commit_message>
<xml_diff>
--- a/notes/Filter API.xlsx
+++ b/notes/Filter API.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-3200" yWindow="-23540" windowWidth="32000" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>DefaultFilter.js</t>
   </si>
@@ -57,15 +57,6 @@
   </si>
   <si>
     <t>set up</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>coumn</t>
-  </si>
-  <si>
-    <t>table</t>
   </si>
   <si>
     <t>module</t>
@@ -1121,6 +1112,64 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>column state</t>
+  </si>
+  <si>
+    <t>"table" state</t>
+  </si>
+  <si>
+    <t>grid state</t>
+  </si>
+  <si>
+    <r>
+      <t>columnFilters.setState(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>state, options</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>columnFilters.getState(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>options</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Lucida Console"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>all columns state</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1427,10 +1476,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1709,15 +1755,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" style="34" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="34" customWidth="1"/>
     <col min="2" max="2" width="28" style="3" customWidth="1"/>
     <col min="3" max="4" width="27.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="36.5" style="22" customWidth="1"/>
@@ -1728,22 +1774,22 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>3</v>
@@ -1751,7 +1797,7 @@
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -1772,21 +1818,21 @@
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1" ht="104" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1806,7 +1852,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G4" s="26" t="s">
         <v>4</v>
@@ -1814,19 +1860,19 @@
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G5" s="29" t="s">
         <v>4</v>
@@ -1834,26 +1880,26 @@
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="34" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>4</v>
@@ -1869,7 +1915,7 @@
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1888,137 +1934,164 @@
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="34" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>30</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
       <c r="E11" s="19" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>36</v>
-      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="20" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>40</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="25"/>
       <c r="G13" s="25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C15" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="27" t="s">
+      <c r="D15" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="28"/>
+      <c r="E15" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="35"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="28"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
-        <v>46</v>
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="34"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>